<commit_message>
Added round 3 bids
</commit_message>
<xml_diff>
--- a/database/seeds/users.xlsx
+++ b/database/seeds/users.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE34C97-FC66-A640-BAF5-DC5ABAAF99A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194D5908-E769-8A49-AAAF-ADAFA64C5D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="580" windowWidth="28800" windowHeight="16240" xr2:uid="{8DAFC702-1F3B-F547-BEBA-3024C546E2F5}"/>
+    <workbookView xWindow="9980" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{8DAFC702-1F3B-F547-BEBA-3024C546E2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">users!$B$1:$C$406</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">users!$B$1:$B$406</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="821">
   <si>
     <t>id</t>
   </si>
@@ -2860,12 +2860,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="8" width="10.83203125" style="1"/>
     <col min="9" max="16384" width="14.5" style="1"/>
@@ -3023,8 +3023,8 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>820</v>
+      <c r="H6" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3049,8 +3049,8 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>820</v>
+      <c r="H7" s="1">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3725,8 +3725,8 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>820</v>
+      <c r="H33" s="1">
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3777,8 +3777,8 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>820</v>
+      <c r="H35" s="1">
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4427,8 +4427,8 @@
       <c r="G60" s="1">
         <v>0</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>820</v>
+      <c r="H60" s="1">
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4479,8 +4479,8 @@
       <c r="G62" s="1">
         <v>0</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>820</v>
+      <c r="H62" s="1">
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4505,8 +4505,8 @@
       <c r="G63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>820</v>
+      <c r="H63" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4869,8 +4869,8 @@
       <c r="G77" s="1">
         <v>1</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>820</v>
+      <c r="H77" s="1">
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4921,8 +4921,8 @@
       <c r="G79" s="1">
         <v>1</v>
       </c>
-      <c r="H79" s="1" t="s">
-        <v>820</v>
+      <c r="H79" s="1">
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4973,8 +4973,8 @@
       <c r="G81" s="1">
         <v>0</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>820</v>
+      <c r="H81" s="1">
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5259,8 +5259,8 @@
       <c r="G92" s="1">
         <v>0</v>
       </c>
-      <c r="H92" s="1" t="s">
-        <v>820</v>
+      <c r="H92" s="1">
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5311,8 +5311,8 @@
       <c r="G94" s="1">
         <v>0</v>
       </c>
-      <c r="H94" s="1" t="s">
-        <v>820</v>
+      <c r="H94" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5696,13 +5696,13 @@
         <v>1</v>
       </c>
       <c r="F109" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G109" s="1">
         <v>0</v>
       </c>
-      <c r="H109" s="1" t="s">
-        <v>820</v>
+      <c r="H109" s="1">
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5727,8 +5727,8 @@
       <c r="G110" s="1">
         <v>0</v>
       </c>
-      <c r="H110" s="1" t="s">
-        <v>820</v>
+      <c r="H110" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5857,8 +5857,8 @@
       <c r="G115" s="1">
         <v>0</v>
       </c>
-      <c r="H115" s="1" t="s">
-        <v>820</v>
+      <c r="H115" s="1">
+        <v>65</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5909,8 +5909,8 @@
       <c r="G117" s="1">
         <v>1</v>
       </c>
-      <c r="H117" s="1" t="s">
-        <v>820</v>
+      <c r="H117" s="1">
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5987,8 +5987,8 @@
       <c r="G120" s="1">
         <v>1</v>
       </c>
-      <c r="H120" s="1" t="s">
-        <v>820</v>
+      <c r="H120" s="1">
+        <v>94</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6065,8 +6065,8 @@
       <c r="G123" s="1">
         <v>0</v>
       </c>
-      <c r="H123" s="1" t="s">
-        <v>820</v>
+      <c r="H123" s="1">
+        <v>66</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6247,8 +6247,8 @@
       <c r="G130" s="1">
         <v>0</v>
       </c>
-      <c r="H130" s="1" t="s">
-        <v>820</v>
+      <c r="H130" s="1">
+        <v>88</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6273,8 +6273,8 @@
       <c r="G131" s="1">
         <v>0</v>
       </c>
-      <c r="H131" s="1" t="s">
-        <v>820</v>
+      <c r="H131" s="1">
+        <v>62</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6299,8 +6299,8 @@
       <c r="G132" s="1">
         <v>0</v>
       </c>
-      <c r="H132" s="1" t="s">
-        <v>820</v>
+      <c r="H132" s="1">
+        <v>72</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6320,7 +6320,7 @@
         <v>0</v>
       </c>
       <c r="F133" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
@@ -6351,8 +6351,8 @@
       <c r="G134" s="1">
         <v>0</v>
       </c>
-      <c r="H134" s="1" t="s">
-        <v>820</v>
+      <c r="H134" s="1">
+        <v>70</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6377,8 +6377,8 @@
       <c r="G135" s="1">
         <v>0</v>
       </c>
-      <c r="H135" s="1" t="s">
-        <v>820</v>
+      <c r="H135" s="1">
+        <v>92</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6429,8 +6429,8 @@
       <c r="G137" s="1">
         <v>0</v>
       </c>
-      <c r="H137" s="1" t="s">
-        <v>820</v>
+      <c r="H137" s="1">
+        <v>91</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6455,8 +6455,8 @@
       <c r="G138" s="1">
         <v>0</v>
       </c>
-      <c r="H138" s="1" t="s">
-        <v>820</v>
+      <c r="H138" s="1">
+        <v>31</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6481,8 +6481,8 @@
       <c r="G139" s="1">
         <v>0</v>
       </c>
-      <c r="H139" s="1" t="s">
-        <v>820</v>
+      <c r="H139" s="1">
+        <v>39</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6507,8 +6507,8 @@
       <c r="G140" s="1">
         <v>0</v>
       </c>
-      <c r="H140" s="1" t="s">
-        <v>820</v>
+      <c r="H140" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6767,8 +6767,8 @@
       <c r="G150" s="1">
         <v>0</v>
       </c>
-      <c r="H150" s="1" t="s">
-        <v>820</v>
+      <c r="H150" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6819,8 +6819,8 @@
       <c r="G152" s="1">
         <v>0</v>
       </c>
-      <c r="H152" s="1" t="s">
-        <v>820</v>
+      <c r="H152" s="1">
+        <v>35</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6845,8 +6845,8 @@
       <c r="G153" s="1">
         <v>1</v>
       </c>
-      <c r="H153" s="1" t="s">
-        <v>820</v>
+      <c r="H153" s="1">
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6949,8 +6949,8 @@
       <c r="G157" s="1">
         <v>0</v>
       </c>
-      <c r="H157" s="1" t="s">
-        <v>820</v>
+      <c r="H157" s="1">
+        <v>41</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7079,8 +7079,8 @@
       <c r="G162" s="1">
         <v>0</v>
       </c>
-      <c r="H162" s="1" t="s">
-        <v>820</v>
+      <c r="H162" s="1">
+        <v>64</v>
       </c>
     </row>
     <row r="163" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7105,8 +7105,8 @@
       <c r="G163" s="1">
         <v>1</v>
       </c>
-      <c r="H163" s="1" t="s">
-        <v>820</v>
+      <c r="H163" s="1">
+        <v>75</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7781,8 +7781,8 @@
       <c r="G189" s="1">
         <v>0</v>
       </c>
-      <c r="H189" s="1" t="s">
-        <v>820</v>
+      <c r="H189" s="1">
+        <v>64</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7807,8 +7807,8 @@
       <c r="G190" s="1">
         <v>0</v>
       </c>
-      <c r="H190" s="1" t="s">
-        <v>820</v>
+      <c r="H190" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="191" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7833,8 +7833,8 @@
       <c r="G191" s="1">
         <v>0</v>
       </c>
-      <c r="H191" s="1" t="s">
-        <v>820</v>
+      <c r="H191" s="1">
+        <v>67</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7859,8 +7859,8 @@
       <c r="G192" s="1">
         <v>0</v>
       </c>
-      <c r="H192" s="1" t="s">
-        <v>820</v>
+      <c r="H192" s="1">
+        <v>96</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7885,8 +7885,8 @@
       <c r="G193" s="1">
         <v>0</v>
       </c>
-      <c r="H193" s="1" t="s">
-        <v>820</v>
+      <c r="H193" s="1">
+        <v>38</v>
       </c>
     </row>
     <row r="194" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8171,8 +8171,8 @@
       <c r="G204" s="1">
         <v>0</v>
       </c>
-      <c r="H204" s="1" t="s">
-        <v>820</v>
+      <c r="H204" s="1">
+        <v>78</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8223,8 +8223,8 @@
       <c r="G206" s="1">
         <v>1</v>
       </c>
-      <c r="H206" s="1" t="s">
-        <v>820</v>
+      <c r="H206" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="207" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8249,8 +8249,8 @@
       <c r="G207" s="1">
         <v>0</v>
       </c>
-      <c r="H207" s="1" t="s">
-        <v>820</v>
+      <c r="H207" s="1">
+        <v>38</v>
       </c>
     </row>
     <row r="208" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8353,8 +8353,8 @@
       <c r="G211" s="1">
         <v>0</v>
       </c>
-      <c r="H211" s="1" t="s">
-        <v>820</v>
+      <c r="H211" s="1">
+        <v>99</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8405,8 +8405,8 @@
       <c r="G213" s="1">
         <v>0</v>
       </c>
-      <c r="H213" s="1" t="s">
-        <v>820</v>
+      <c r="H213" s="1">
+        <v>35</v>
       </c>
     </row>
     <row r="214" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8561,8 +8561,8 @@
       <c r="G219" s="1">
         <v>1</v>
       </c>
-      <c r="H219" s="1" t="s">
-        <v>820</v>
+      <c r="H219" s="1">
+        <v>74</v>
       </c>
     </row>
     <row r="220" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8587,8 +8587,8 @@
       <c r="G220" s="1">
         <v>0</v>
       </c>
-      <c r="H220" s="1" t="s">
-        <v>820</v>
+      <c r="H220" s="1">
+        <v>42</v>
       </c>
     </row>
     <row r="221" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8613,8 +8613,8 @@
       <c r="G221" s="1">
         <v>0</v>
       </c>
-      <c r="H221" s="1" t="s">
-        <v>820</v>
+      <c r="H221" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="222" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8639,8 +8639,8 @@
       <c r="G222" s="1">
         <v>0</v>
       </c>
-      <c r="H222" s="1" t="s">
-        <v>820</v>
+      <c r="H222" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8665,8 +8665,8 @@
       <c r="G223" s="1">
         <v>0</v>
       </c>
-      <c r="H223" s="1" t="s">
-        <v>820</v>
+      <c r="H223" s="1">
+        <v>39</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8691,8 +8691,8 @@
       <c r="G224" s="1">
         <v>0</v>
       </c>
-      <c r="H224" s="1" t="s">
-        <v>820</v>
+      <c r="H224" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="225" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8795,8 +8795,8 @@
       <c r="G228" s="1">
         <v>0</v>
       </c>
-      <c r="H228" s="1" t="s">
-        <v>820</v>
+      <c r="H228" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8821,8 +8821,8 @@
       <c r="G229" s="1">
         <v>0</v>
       </c>
-      <c r="H229" s="1" t="s">
-        <v>820</v>
+      <c r="H229" s="1">
+        <v>99</v>
       </c>
     </row>
     <row r="230" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8847,8 +8847,8 @@
       <c r="G230" s="1">
         <v>1</v>
       </c>
-      <c r="H230" s="1" t="s">
-        <v>820</v>
+      <c r="H230" s="1">
+        <v>79</v>
       </c>
     </row>
     <row r="231" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9003,8 +9003,8 @@
       <c r="G236" s="1">
         <v>1</v>
       </c>
-      <c r="H236" s="1" t="s">
-        <v>820</v>
+      <c r="H236" s="1">
+        <v>47</v>
       </c>
     </row>
     <row r="237" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9081,8 +9081,8 @@
       <c r="G239" s="1">
         <v>0</v>
       </c>
-      <c r="H239" s="1" t="s">
-        <v>820</v>
+      <c r="H239" s="1">
+        <v>23</v>
       </c>
     </row>
     <row r="240" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9107,8 +9107,8 @@
       <c r="G240" s="1">
         <v>0</v>
       </c>
-      <c r="H240" s="1" t="s">
-        <v>820</v>
+      <c r="H240" s="1">
+        <v>35</v>
       </c>
     </row>
     <row r="241" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9159,8 +9159,8 @@
       <c r="G242" s="1">
         <v>0</v>
       </c>
-      <c r="H242" s="1" t="s">
-        <v>820</v>
+      <c r="H242" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9211,8 +9211,8 @@
       <c r="G244" s="1">
         <v>1</v>
       </c>
-      <c r="H244" s="1" t="s">
-        <v>820</v>
+      <c r="H244" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -9315,8 +9315,8 @@
       <c r="G248" s="1">
         <v>0</v>
       </c>
-      <c r="H248" s="1" t="s">
-        <v>820</v>
+      <c r="H248" s="1">
+        <v>43</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10225,8 +10225,8 @@
       <c r="G283" s="1">
         <v>1</v>
       </c>
-      <c r="H283" s="1" t="s">
-        <v>820</v>
+      <c r="H283" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="284" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10381,8 +10381,8 @@
       <c r="G289" s="1">
         <v>0</v>
       </c>
-      <c r="H289" s="1" t="s">
-        <v>820</v>
+      <c r="H289" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="290" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10485,8 +10485,8 @@
       <c r="G293" s="1">
         <v>0</v>
       </c>
-      <c r="H293" s="1" t="s">
-        <v>820</v>
+      <c r="H293" s="1">
+        <v>40</v>
       </c>
     </row>
     <row r="294" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10537,8 +10537,8 @@
       <c r="G295" s="1">
         <v>0</v>
       </c>
-      <c r="H295" s="1" t="s">
-        <v>820</v>
+      <c r="H295" s="1">
+        <v>77</v>
       </c>
     </row>
     <row r="296" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10563,8 +10563,8 @@
       <c r="G296" s="1">
         <v>0</v>
       </c>
-      <c r="H296" s="1" t="s">
-        <v>820</v>
+      <c r="H296" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="297" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10615,8 +10615,8 @@
       <c r="G298" s="1">
         <v>1</v>
       </c>
-      <c r="H298" s="1" t="s">
-        <v>820</v>
+      <c r="H298" s="1">
+        <v>72</v>
       </c>
     </row>
     <row r="299" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10641,8 +10641,8 @@
       <c r="G299" s="1">
         <v>0</v>
       </c>
-      <c r="H299" s="1" t="s">
-        <v>820</v>
+      <c r="H299" s="1">
+        <v>43</v>
       </c>
     </row>
     <row r="300" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10667,8 +10667,8 @@
       <c r="G300" s="1">
         <v>0</v>
       </c>
-      <c r="H300" s="1" t="s">
-        <v>820</v>
+      <c r="H300" s="1">
+        <v>53</v>
       </c>
     </row>
     <row r="301" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10693,8 +10693,8 @@
       <c r="G301" s="1">
         <v>0</v>
       </c>
-      <c r="H301" s="1" t="s">
-        <v>820</v>
+      <c r="H301" s="1">
+        <v>23</v>
       </c>
     </row>
     <row r="302" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10745,8 +10745,8 @@
       <c r="G303" s="1">
         <v>0</v>
       </c>
-      <c r="H303" s="1" t="s">
-        <v>820</v>
+      <c r="H303" s="1">
+        <v>84</v>
       </c>
     </row>
     <row r="304" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10771,8 +10771,8 @@
       <c r="G304" s="1">
         <v>1</v>
       </c>
-      <c r="H304" s="1" t="s">
-        <v>820</v>
+      <c r="H304" s="1">
+        <v>51</v>
       </c>
     </row>
     <row r="305" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10849,8 +10849,8 @@
       <c r="G307" s="1">
         <v>0</v>
       </c>
-      <c r="H307" s="1" t="s">
-        <v>820</v>
+      <c r="H307" s="1">
+        <v>24</v>
       </c>
     </row>
     <row r="308" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10979,8 +10979,8 @@
       <c r="G312" s="1">
         <v>1</v>
       </c>
-      <c r="H312" s="1" t="s">
-        <v>820</v>
+      <c r="H312" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="313" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11031,8 +11031,8 @@
       <c r="G314" s="1">
         <v>1</v>
       </c>
-      <c r="H314" s="1" t="s">
-        <v>820</v>
+      <c r="H314" s="1">
+        <v>58</v>
       </c>
     </row>
     <row r="315" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11213,8 +11213,8 @@
       <c r="G321" s="1">
         <v>0</v>
       </c>
-      <c r="H321" s="1" t="s">
-        <v>820</v>
+      <c r="H321" s="1">
+        <v>87</v>
       </c>
     </row>
     <row r="322" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11265,8 +11265,8 @@
       <c r="G323" s="1">
         <v>0</v>
       </c>
-      <c r="H323" s="1" t="s">
-        <v>820</v>
+      <c r="H323" s="1">
+        <v>34</v>
       </c>
     </row>
     <row r="324" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11317,8 +11317,8 @@
       <c r="G325" s="1">
         <v>0</v>
       </c>
-      <c r="H325" s="1" t="s">
-        <v>820</v>
+      <c r="H325" s="1">
+        <v>19</v>
       </c>
     </row>
     <row r="326" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11343,8 +11343,8 @@
       <c r="G326" s="1">
         <v>0</v>
       </c>
-      <c r="H326" s="1" t="s">
-        <v>820</v>
+      <c r="H326" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="327" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -11647,7 +11647,7 @@
         <v>678</v>
       </c>
       <c r="E338" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F338" s="1">
         <v>3</v>
@@ -11655,8 +11655,8 @@
       <c r="G338" s="1">
         <v>1</v>
       </c>
-      <c r="H338" s="1" t="s">
-        <v>820</v>
+      <c r="H338" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="339" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12305,8 +12305,8 @@
       <c r="G363" s="1">
         <v>0</v>
       </c>
-      <c r="H363" s="1" t="s">
-        <v>820</v>
+      <c r="H363" s="1">
+        <v>18</v>
       </c>
     </row>
     <row r="364" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12383,8 +12383,8 @@
       <c r="G366" s="1">
         <v>0</v>
       </c>
-      <c r="H366" s="1" t="s">
-        <v>820</v>
+      <c r="H366" s="1">
+        <v>47</v>
       </c>
     </row>
     <row r="367" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12409,8 +12409,8 @@
       <c r="G367" s="1">
         <v>0</v>
       </c>
-      <c r="H367" s="1" t="s">
-        <v>820</v>
+      <c r="H367" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="368" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12643,8 +12643,8 @@
       <c r="G376" s="1">
         <v>1</v>
       </c>
-      <c r="H376" s="1" t="s">
-        <v>820</v>
+      <c r="H376" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="377" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12695,8 +12695,8 @@
       <c r="G378" s="1">
         <v>1</v>
       </c>
-      <c r="H378" s="1" t="s">
-        <v>820</v>
+      <c r="H378" s="1">
+        <v>31</v>
       </c>
     </row>
     <row r="379" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12747,8 +12747,8 @@
       <c r="G380" s="1">
         <v>1</v>
       </c>
-      <c r="H380" s="1" t="s">
-        <v>820</v>
+      <c r="H380" s="1">
+        <v>78</v>
       </c>
     </row>
     <row r="381" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12799,8 +12799,8 @@
       <c r="G382" s="1">
         <v>0</v>
       </c>
-      <c r="H382" s="1" t="s">
-        <v>820</v>
+      <c r="H382" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="383" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12851,8 +12851,8 @@
       <c r="G384" s="1">
         <v>0</v>
       </c>
-      <c r="H384" s="1" t="s">
-        <v>820</v>
+      <c r="H384" s="1">
+        <v>57</v>
       </c>
     </row>
     <row r="385" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12903,8 +12903,8 @@
       <c r="G386" s="1">
         <v>0</v>
       </c>
-      <c r="H386" s="1" t="s">
-        <v>820</v>
+      <c r="H386" s="1">
+        <v>97</v>
       </c>
     </row>
     <row r="387" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -12981,8 +12981,8 @@
       <c r="G389" s="1">
         <v>0</v>
       </c>
-      <c r="H389" s="1" t="s">
-        <v>820</v>
+      <c r="H389" s="1">
+        <v>44</v>
       </c>
     </row>
     <row r="390" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -13007,8 +13007,8 @@
       <c r="G390" s="1">
         <v>0</v>
       </c>
-      <c r="H390" s="1" t="s">
-        <v>820</v>
+      <c r="H390" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="391" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -13059,8 +13059,8 @@
       <c r="G392" s="1">
         <v>0</v>
       </c>
-      <c r="H392" s="1" t="s">
-        <v>820</v>
+      <c r="H392" s="1">
+        <v>69</v>
       </c>
     </row>
     <row r="393" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -13345,8 +13345,8 @@
       <c r="G403" s="1">
         <v>0</v>
       </c>
-      <c r="H403" s="1" t="s">
-        <v>820</v>
+      <c r="H403" s="1">
+        <v>23</v>
       </c>
     </row>
     <row r="404" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -13397,8 +13397,8 @@
       <c r="G405" s="1">
         <v>1</v>
       </c>
-      <c r="H405" s="1" t="s">
-        <v>820</v>
+      <c r="H405" s="1">
+        <v>99</v>
       </c>
     </row>
     <row r="406" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix round 3 allocations
</commit_message>
<xml_diff>
--- a/database/seeds/users.xlsx
+++ b/database/seeds/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194D5908-E769-8A49-AAAF-ADAFA64C5D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD500B26-595F-E74A-8E6A-6FCE6C1D109D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{8DAFC702-1F3B-F547-BEBA-3024C546E2F5}"/>
+    <workbookView xWindow="9600" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{8DAFC702-1F3B-F547-BEBA-3024C546E2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -2859,8 +2859,8 @@
   <dimension ref="A1:H406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H296" sqref="H296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10564,7 +10564,7 @@
         <v>0</v>
       </c>
       <c r="H296" s="1">
-        <v>13</v>
+        <v>71</v>
       </c>
     </row>
     <row r="297" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -10694,7 +10694,7 @@
         <v>0</v>
       </c>
       <c r="H301" s="1">
-        <v>23</v>
+        <v>67</v>
       </c>
     </row>
     <row r="302" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>